<commit_message>
Atualização dos gráficos 26082020
</commit_message>
<xml_diff>
--- a/Sistema-Operacional/Entradas/Monitoramento_Mananciais_Criticos.xlsx
+++ b/Sistema-Operacional/Entradas/Monitoramento_Mananciais_Criticos.xlsx
@@ -31,10 +31,10 @@
     <t>AN_TRI_202008</t>
   </si>
   <si>
-    <t>AC_20200816</t>
-  </si>
-  <si>
-    <t>AN_20200816</t>
+    <t>AC_20200823</t>
+  </si>
+  <si>
+    <t>AN_20200823</t>
   </si>
   <si>
     <t>SPI1_202007</t>
@@ -569,19 +569,19 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>-11.3</v>
+        <v>-8.3</v>
       </c>
       <c r="D2">
-        <v>-12</v>
+        <v>-4.9</v>
       </c>
       <c r="E2">
-        <v>11.7</v>
+        <v>30.7</v>
       </c>
       <c r="F2">
-        <v>78.1</v>
+        <v>130.7</v>
       </c>
       <c r="G2">
-        <v>-15</v>
+        <v>42.3</v>
       </c>
       <c r="H2">
         <v>-0.64</v>
@@ -604,19 +604,19 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>-7.3</v>
+        <v>-4.2</v>
       </c>
       <c r="D3">
-        <v>-1</v>
+        <v>6.7</v>
       </c>
       <c r="E3">
-        <v>31.5</v>
+        <v>52.1</v>
       </c>
       <c r="F3">
-        <v>89.4</v>
+        <v>145.2</v>
       </c>
       <c r="G3">
-        <v>-12.1</v>
+        <v>42.7</v>
       </c>
       <c r="H3">
         <v>-0.71</v>
@@ -639,19 +639,19 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>-10.4</v>
+        <v>-7.1</v>
       </c>
       <c r="D4">
-        <v>-6.1</v>
+        <v>1.7</v>
       </c>
       <c r="E4">
-        <v>-0.3</v>
+        <v>18.6</v>
       </c>
       <c r="F4">
-        <v>84.3</v>
+        <v>132.1</v>
       </c>
       <c r="G4">
-        <v>33.6</v>
+        <v>109.4</v>
       </c>
       <c r="H4">
         <v>-0.52</v>
@@ -674,19 +674,19 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>-29.1</v>
+        <v>-24.9</v>
       </c>
       <c r="D5">
-        <v>-22</v>
+        <v>-11</v>
       </c>
       <c r="E5">
-        <v>-5.8</v>
+        <v>22.5</v>
       </c>
       <c r="F5">
-        <v>72.4</v>
+        <v>142.3</v>
       </c>
       <c r="G5">
-        <v>-25.4</v>
+        <v>46.7</v>
       </c>
       <c r="H5">
         <v>-1.73</v>
@@ -709,19 +709,19 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>-26.7</v>
+        <v>-23.1</v>
       </c>
       <c r="D6">
-        <v>-31.1</v>
+        <v>-22.9</v>
       </c>
       <c r="E6">
-        <v>-29.2</v>
+        <v>-9.1</v>
       </c>
       <c r="F6">
-        <v>76.5</v>
+        <v>136.6</v>
       </c>
       <c r="G6">
-        <v>-20.5</v>
+        <v>41.9</v>
       </c>
       <c r="H6">
         <v>-0.52</v>
@@ -744,19 +744,19 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>-25.2</v>
+        <v>-21.2</v>
       </c>
       <c r="D7">
-        <v>-31.2</v>
+        <v>-22.2</v>
       </c>
       <c r="E7">
-        <v>-31</v>
+        <v>-11.5</v>
       </c>
       <c r="F7">
-        <v>62.5</v>
+        <v>137.6</v>
       </c>
       <c r="G7">
-        <v>-36</v>
+        <v>40.8</v>
       </c>
       <c r="H7">
         <v>-0.95</v>
@@ -779,19 +779,19 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>-54.3</v>
+        <v>-49.3</v>
       </c>
       <c r="D8">
-        <v>-49.8</v>
+        <v>-37.2</v>
       </c>
       <c r="E8">
-        <v>-20.5</v>
+        <v>5.8</v>
       </c>
       <c r="F8">
-        <v>73.3</v>
+        <v>151.1</v>
       </c>
       <c r="G8">
-        <v>-12.9</v>
+        <v>79.4</v>
       </c>
       <c r="H8">
         <v>-1.39</v>
@@ -814,19 +814,19 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>-17.9</v>
+        <v>-15.9</v>
       </c>
       <c r="D9">
-        <v>-6.9</v>
+        <v>-2.3</v>
       </c>
       <c r="E9">
-        <v>25.6</v>
+        <v>38.2</v>
       </c>
       <c r="F9">
-        <v>87.6</v>
+        <v>123.1</v>
       </c>
       <c r="G9">
-        <v>-21</v>
+        <v>11</v>
       </c>
       <c r="H9">
         <v>-0.59</v>
@@ -849,19 +849,19 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>-20.8</v>
+        <v>-16.8</v>
       </c>
       <c r="D10">
-        <v>-27.4</v>
+        <v>-18.2</v>
       </c>
       <c r="E10">
-        <v>-20.6</v>
+        <v>2.2</v>
       </c>
       <c r="F10">
-        <v>90.7</v>
+        <v>155.9</v>
       </c>
       <c r="G10">
-        <v>-5.7</v>
+        <v>62</v>
       </c>
       <c r="H10">
         <v>-0.47</v>
@@ -884,19 +884,19 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>-14</v>
+        <v>-10.5</v>
       </c>
       <c r="D11">
-        <v>-19.7</v>
+        <v>-11.6</v>
       </c>
       <c r="E11">
-        <v>-15.2</v>
+        <v>6.2</v>
       </c>
       <c r="F11">
-        <v>71.2</v>
+        <v>132.3</v>
       </c>
       <c r="G11">
-        <v>-7.5</v>
+        <v>72</v>
       </c>
       <c r="H11">
         <v>-0.54</v>
@@ -919,19 +919,19 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>-14.4</v>
+        <v>-11.1</v>
       </c>
       <c r="D12">
-        <v>-19.9</v>
+        <v>-12.1</v>
       </c>
       <c r="E12">
-        <v>-11.9</v>
+        <v>8.6</v>
       </c>
       <c r="F12">
-        <v>74.9</v>
+        <v>132.6</v>
       </c>
       <c r="G12">
-        <v>-3.3</v>
+        <v>71.2</v>
       </c>
       <c r="H12">
         <v>-0.54</v>
@@ -954,19 +954,19 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>-13.5</v>
+        <v>-10.5</v>
       </c>
       <c r="D13">
-        <v>-18.3</v>
+        <v>-11.1</v>
       </c>
       <c r="E13">
-        <v>-0.6</v>
+        <v>18.7</v>
       </c>
       <c r="F13">
-        <v>74.6</v>
+        <v>129.5</v>
       </c>
       <c r="G13">
-        <v>-12.7</v>
+        <v>51.5</v>
       </c>
       <c r="H13">
         <v>-0.63</v>
@@ -989,19 +989,19 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>-21.9</v>
+        <v>-19.8</v>
       </c>
       <c r="D14">
-        <v>-21.6</v>
+        <v>-16.6</v>
       </c>
       <c r="E14">
-        <v>10.4</v>
+        <v>23.2</v>
       </c>
       <c r="F14">
-        <v>71.4</v>
+        <v>108.8</v>
       </c>
       <c r="G14">
-        <v>-26</v>
+        <v>12.8</v>
       </c>
       <c r="H14">
         <v>-0.64</v>
@@ -1024,19 +1024,19 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>-31.8</v>
+        <v>-25</v>
       </c>
       <c r="D15">
-        <v>-40.5</v>
+        <v>-21.5</v>
       </c>
       <c r="E15">
-        <v>-23.5</v>
+        <v>26</v>
       </c>
       <c r="F15">
-        <v>39.7</v>
+        <v>138.1</v>
       </c>
       <c r="G15">
-        <v>-36</v>
+        <v>122.6</v>
       </c>
       <c r="H15">
         <v>-1.42</v>
@@ -1059,19 +1059,19 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>-5.6</v>
+        <v>-2.6</v>
       </c>
       <c r="D16">
-        <v>3.1</v>
+        <v>10.6</v>
       </c>
       <c r="E16">
-        <v>36.6</v>
+        <v>56.7</v>
       </c>
       <c r="F16">
-        <v>92.2</v>
+        <v>146.6</v>
       </c>
       <c r="G16">
-        <v>-13.8</v>
+        <v>37</v>
       </c>
       <c r="H16">
         <v>-0.69</v>
@@ -1094,19 +1094,19 @@
         <v>26</v>
       </c>
       <c r="C17">
-        <v>-17.3</v>
+        <v>-15.1</v>
       </c>
       <c r="D17">
-        <v>-9.5</v>
+        <v>-4</v>
       </c>
       <c r="E17">
-        <v>21.1</v>
+        <v>35.7</v>
       </c>
       <c r="F17">
-        <v>89</v>
+        <v>131.5</v>
       </c>
       <c r="G17">
-        <v>-17.2</v>
+        <v>22.2</v>
       </c>
       <c r="H17">
         <v>-0.68</v>
@@ -1129,19 +1129,19 @@
         <v>27</v>
       </c>
       <c r="C18">
-        <v>-29.6</v>
+        <v>-26.4</v>
       </c>
       <c r="D18">
-        <v>-34</v>
+        <v>-26.5</v>
       </c>
       <c r="E18">
-        <v>-26.6</v>
+        <v>-8.2</v>
       </c>
       <c r="F18">
-        <v>100</v>
+        <v>156.6</v>
       </c>
       <c r="G18">
-        <v>33</v>
+        <v>108.2</v>
       </c>
       <c r="H18">
         <v>-0.48</v>
@@ -1164,19 +1164,19 @@
         <v>28</v>
       </c>
       <c r="C19">
-        <v>-18.1</v>
+        <v>-14.8</v>
       </c>
       <c r="D19">
-        <v>-22.6</v>
+        <v>-14.9</v>
       </c>
       <c r="E19">
-        <v>-19</v>
+        <v>1.1</v>
       </c>
       <c r="F19">
-        <v>71.7</v>
+        <v>133.6</v>
       </c>
       <c r="G19">
-        <v>-16.1</v>
+        <v>56.3</v>
       </c>
       <c r="H19">
         <v>-0.76</v>
@@ -1199,19 +1199,19 @@
         <v>29</v>
       </c>
       <c r="C20">
-        <v>-45.2</v>
+        <v>-41.3</v>
       </c>
       <c r="D20">
-        <v>-56.8</v>
+        <v>-47.5</v>
       </c>
       <c r="E20">
-        <v>-42.3</v>
+        <v>-24.5</v>
       </c>
       <c r="F20">
-        <v>62.6</v>
+        <v>130.1</v>
       </c>
       <c r="G20">
-        <v>-26.4</v>
+        <v>53.1</v>
       </c>
       <c r="H20">
         <v>-1.11</v>
@@ -1234,19 +1234,19 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>-26.2</v>
+        <v>-17.9</v>
       </c>
       <c r="D21">
-        <v>-33</v>
+        <v>-10.9</v>
       </c>
       <c r="E21">
-        <v>-24.2</v>
+        <v>30.6</v>
       </c>
       <c r="F21">
-        <v>45</v>
+        <v>175.2</v>
       </c>
       <c r="G21">
-        <v>-27.2</v>
+        <v>183.7</v>
       </c>
       <c r="H21">
         <v>-1.14</v>
@@ -1269,19 +1269,19 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>-39.6</v>
+        <v>-33.6</v>
       </c>
       <c r="D22">
-        <v>-42.5</v>
+        <v>-26.3</v>
       </c>
       <c r="E22">
-        <v>-34.4</v>
+        <v>6.5</v>
       </c>
       <c r="F22">
-        <v>57</v>
+        <v>178.6</v>
       </c>
       <c r="G22">
-        <v>-34.2</v>
+        <v>106.3</v>
       </c>
       <c r="H22">
         <v>-1.14</v>
@@ -1304,19 +1304,19 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>-29.1</v>
+        <v>-24.6</v>
       </c>
       <c r="D23">
-        <v>-32</v>
+        <v>-21.9</v>
       </c>
       <c r="E23">
-        <v>-32.4</v>
+        <v>-10.9</v>
       </c>
       <c r="F23">
-        <v>66.7</v>
+        <v>146.4</v>
       </c>
       <c r="G23">
-        <v>-26</v>
+        <v>62.2</v>
       </c>
       <c r="H23">
         <v>-0.68</v>
@@ -1339,19 +1339,19 @@
         <v>32</v>
       </c>
       <c r="C24">
-        <v>-52.8</v>
+        <v>-50</v>
       </c>
       <c r="D24">
-        <v>-53.8</v>
+        <v>-46</v>
       </c>
       <c r="E24">
-        <v>-28.6</v>
+        <v>-10.6</v>
       </c>
       <c r="F24">
-        <v>55.7</v>
+        <v>107</v>
       </c>
       <c r="G24">
-        <v>-40</v>
+        <v>15.3</v>
       </c>
       <c r="H24">
         <v>-1.28</v>
@@ -1374,19 +1374,19 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <v>-54.8</v>
+        <v>-52.1</v>
       </c>
       <c r="D25">
-        <v>-54.9</v>
+        <v>-47.3</v>
       </c>
       <c r="E25">
-        <v>-29.7</v>
+        <v>-12.1</v>
       </c>
       <c r="F25">
-        <v>58</v>
+        <v>111.7</v>
       </c>
       <c r="G25">
-        <v>-42.5</v>
+        <v>10.7</v>
       </c>
       <c r="H25">
         <v>-1.29</v>
@@ -1409,19 +1409,19 @@
         <v>34</v>
       </c>
       <c r="C26">
-        <v>-48.6</v>
+        <v>-45.5</v>
       </c>
       <c r="D26">
-        <v>-46.3</v>
+        <v>-37.7</v>
       </c>
       <c r="E26">
-        <v>-19</v>
+        <v>0.7</v>
       </c>
       <c r="F26">
-        <v>43.5</v>
+        <v>101.5</v>
       </c>
       <c r="G26">
-        <v>-51.1</v>
+        <v>14</v>
       </c>
       <c r="H26">
         <v>-1.3</v>
@@ -1444,19 +1444,19 @@
         <v>35</v>
       </c>
       <c r="C27">
-        <v>-40.7</v>
+        <v>-32.5</v>
       </c>
       <c r="D27">
-        <v>-44.6</v>
+        <v>-24.2</v>
       </c>
       <c r="E27">
-        <v>-29</v>
+        <v>20.3</v>
       </c>
       <c r="F27">
-        <v>47.2</v>
+        <v>206.5</v>
       </c>
       <c r="G27">
-        <v>-44.2</v>
+        <v>143.8</v>
       </c>
       <c r="H27">
         <v>-1.06</v>
@@ -1479,19 +1479,19 @@
         <v>36</v>
       </c>
       <c r="C28">
-        <v>-29.2</v>
+        <v>-24.9</v>
       </c>
       <c r="D28">
-        <v>-20</v>
+        <v>-9.3</v>
       </c>
       <c r="E28">
-        <v>14.6</v>
+        <v>42.4</v>
       </c>
       <c r="F28">
-        <v>119.4</v>
+        <v>199.3</v>
       </c>
       <c r="G28">
-        <v>19.5</v>
+        <v>99.6</v>
       </c>
       <c r="H28">
         <v>-1.11</v>
@@ -1514,19 +1514,19 @@
         <v>37</v>
       </c>
       <c r="C29">
-        <v>-36.9</v>
+        <v>-30.8</v>
       </c>
       <c r="D29">
-        <v>-41.2</v>
+        <v>-25.7</v>
       </c>
       <c r="E29">
-        <v>-22</v>
+        <v>14.2</v>
       </c>
       <c r="F29">
-        <v>46.9</v>
+        <v>161.5</v>
       </c>
       <c r="G29">
-        <v>-40.4</v>
+        <v>105</v>
       </c>
       <c r="H29">
         <v>-1.14</v>
@@ -1549,19 +1549,19 @@
         <v>38</v>
       </c>
       <c r="C30">
-        <v>-24.9</v>
+        <v>-21.4</v>
       </c>
       <c r="D30">
-        <v>-32.3</v>
+        <v>-23.8</v>
       </c>
       <c r="E30">
-        <v>-32.3</v>
+        <v>-13.4</v>
       </c>
       <c r="F30">
-        <v>83.6</v>
+        <v>140.7</v>
       </c>
       <c r="G30">
-        <v>-6.1</v>
+        <v>57.9</v>
       </c>
       <c r="H30">
         <v>-0.91</v>
@@ -1584,19 +1584,19 @@
         <v>39</v>
       </c>
       <c r="C31">
-        <v>-26.8</v>
+        <v>-23.5</v>
       </c>
       <c r="D31">
-        <v>-36.3</v>
+        <v>-28.7</v>
       </c>
       <c r="E31">
-        <v>-34.2</v>
+        <v>-16.7</v>
       </c>
       <c r="F31">
-        <v>101.3</v>
+        <v>156.6</v>
       </c>
       <c r="G31">
-        <v>3.9</v>
+        <v>60.6</v>
       </c>
       <c r="H31">
         <v>-0.91</v>
@@ -1619,19 +1619,19 @@
         <v>40</v>
       </c>
       <c r="C32">
-        <v>-50</v>
+        <v>-46.5</v>
       </c>
       <c r="D32">
-        <v>-58.5</v>
+        <v>-50.1</v>
       </c>
       <c r="E32">
-        <v>-38.1</v>
+        <v>-20.6</v>
       </c>
       <c r="F32">
-        <v>65.2</v>
+        <v>116.8</v>
       </c>
       <c r="G32">
-        <v>-15.7</v>
+        <v>51</v>
       </c>
       <c r="H32">
         <v>-1.03</v>
@@ -1654,19 +1654,19 @@
         <v>41</v>
       </c>
       <c r="C33">
-        <v>-31.1</v>
+        <v>-26.6</v>
       </c>
       <c r="D33">
-        <v>-43</v>
+        <v>-31.5</v>
       </c>
       <c r="E33">
-        <v>-8.1</v>
+        <v>15.7</v>
       </c>
       <c r="F33">
-        <v>63.5</v>
+        <v>121.1</v>
       </c>
       <c r="G33">
-        <v>44.6</v>
+        <v>175.9</v>
       </c>
       <c r="H33">
         <v>-1.1</v>
@@ -1689,19 +1689,19 @@
         <v>42</v>
       </c>
       <c r="C34">
-        <v>-46.2</v>
+        <v>-44.6</v>
       </c>
       <c r="D34">
-        <v>-51.5</v>
+        <v>-47.6</v>
       </c>
       <c r="E34">
-        <v>-15.2</v>
+        <v>-6.7</v>
       </c>
       <c r="F34">
-        <v>64.9</v>
+        <v>90.9</v>
       </c>
       <c r="G34">
-        <v>-34</v>
+        <v>-7.5</v>
       </c>
       <c r="H34">
         <v>-0.43</v>
@@ -1724,19 +1724,19 @@
         <v>43</v>
       </c>
       <c r="C35">
-        <v>-50.8</v>
+        <v>-48</v>
       </c>
       <c r="D35">
-        <v>-57.1</v>
+        <v>-50.3</v>
       </c>
       <c r="E35">
-        <v>-23.7</v>
+        <v>-8.4</v>
       </c>
       <c r="F35">
-        <v>47.2</v>
+        <v>91.6</v>
       </c>
       <c r="G35">
-        <v>-31.8</v>
+        <v>32.4</v>
       </c>
       <c r="H35">
         <v>-0.49</v>
@@ -1759,19 +1759,19 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>-46.3</v>
+        <v>-43.3</v>
       </c>
       <c r="D36">
-        <v>-53.6</v>
+        <v>-45.8</v>
       </c>
       <c r="E36">
-        <v>-29.4</v>
+        <v>-13</v>
       </c>
       <c r="F36">
-        <v>54.6</v>
+        <v>106.2</v>
       </c>
       <c r="G36">
-        <v>-37.1</v>
+        <v>22.1</v>
       </c>
       <c r="H36">
         <v>-0.64</v>
@@ -1794,19 +1794,19 @@
         <v>45</v>
       </c>
       <c r="C37">
-        <v>-46.1</v>
+        <v>-43.1</v>
       </c>
       <c r="D37">
-        <v>-52.8</v>
+        <v>-44.8</v>
       </c>
       <c r="E37">
-        <v>-29</v>
+        <v>-12.4</v>
       </c>
       <c r="F37">
-        <v>54</v>
+        <v>104.8</v>
       </c>
       <c r="G37">
-        <v>-36.3</v>
+        <v>23.7</v>
       </c>
       <c r="H37">
         <v>-0.67</v>
@@ -1829,19 +1829,19 @@
         <v>46</v>
       </c>
       <c r="C38">
-        <v>-51.5</v>
+        <v>-48.6</v>
       </c>
       <c r="D38">
-        <v>-58.2</v>
+        <v>-51.3</v>
       </c>
       <c r="E38">
-        <v>-25.7</v>
+        <v>-10.3</v>
       </c>
       <c r="F38">
-        <v>46.9</v>
+        <v>94</v>
       </c>
       <c r="G38">
-        <v>-35.1</v>
+        <v>30</v>
       </c>
       <c r="H38">
         <v>-0.5</v>
@@ -1864,19 +1864,19 @@
         <v>47</v>
       </c>
       <c r="C39">
-        <v>-49.4</v>
+        <v>-46.5</v>
       </c>
       <c r="D39">
-        <v>-53.5</v>
+        <v>-46</v>
       </c>
       <c r="E39">
-        <v>-27.3</v>
+        <v>-10.9</v>
       </c>
       <c r="F39">
-        <v>51.9</v>
+        <v>102.2</v>
       </c>
       <c r="G39">
-        <v>-35.5</v>
+        <v>26.9</v>
       </c>
       <c r="H39">
         <v>-0.66</v>
@@ -1899,19 +1899,19 @@
         <v>48</v>
       </c>
       <c r="C40">
-        <v>-59.4</v>
+        <v>-57.5</v>
       </c>
       <c r="D40">
-        <v>-61.9</v>
+        <v>-56.6</v>
       </c>
       <c r="E40">
-        <v>-30.6</v>
+        <v>-18.5</v>
       </c>
       <c r="F40">
-        <v>31.2</v>
+        <v>71.3</v>
       </c>
       <c r="G40">
-        <v>-70.1</v>
+        <v>-31.5</v>
       </c>
       <c r="H40">
         <v>-0.43</v>
@@ -1934,19 +1934,19 @@
         <v>49</v>
       </c>
       <c r="C41">
-        <v>-42.9</v>
+        <v>-38.3</v>
       </c>
       <c r="D41">
-        <v>-53.7</v>
+        <v>-43.2</v>
       </c>
       <c r="E41">
-        <v>-30.2</v>
+        <v>-8.7</v>
       </c>
       <c r="F41">
-        <v>63.3</v>
+        <v>129.8</v>
       </c>
       <c r="G41">
-        <v>-19.8</v>
+        <v>64.4</v>
       </c>
       <c r="H41">
         <v>-1.02</v>
@@ -1969,19 +1969,19 @@
         <v>50</v>
       </c>
       <c r="C42">
-        <v>-32.7</v>
+        <v>-30.6</v>
       </c>
       <c r="D42">
-        <v>-32.7</v>
+        <v>-27.7</v>
       </c>
       <c r="E42">
-        <v>-20.8</v>
+        <v>-8.5</v>
       </c>
       <c r="F42">
-        <v>61.7</v>
+        <v>96.8</v>
       </c>
       <c r="G42">
-        <v>-28.6</v>
+        <v>12.1</v>
       </c>
       <c r="H42">
         <v>-0.51</v>

</xml_diff>

<commit_message>
atualizacao 06 01 2021
</commit_message>
<xml_diff>
--- a/Sistema-Operacional/Entradas/Monitoramento_Mananciais_Criticos.xlsx
+++ b/Sistema-Operacional/Entradas/Monitoramento_Mananciais_Criticos.xlsx
@@ -22,31 +22,31 @@
     <t>MUNICIPIO</t>
   </si>
   <si>
-    <t>AN_ANUAL_202102</t>
-  </si>
-  <si>
-    <t>AN_SEM_202102</t>
-  </si>
-  <si>
-    <t>AN_TRI_202102</t>
-  </si>
-  <si>
-    <t>AC_20210215</t>
-  </si>
-  <si>
-    <t>AN_20210215</t>
-  </si>
-  <si>
-    <t>SPI1_202101</t>
-  </si>
-  <si>
-    <t>SPI3_202101</t>
-  </si>
-  <si>
-    <t>SPI6_202101</t>
-  </si>
-  <si>
-    <t>SPI12_202101</t>
+    <t>AN_ANUAL_202105</t>
+  </si>
+  <si>
+    <t>AN_SEM_202105</t>
+  </si>
+  <si>
+    <t>AN_TRI_202105</t>
+  </si>
+  <si>
+    <t>AC_202105</t>
+  </si>
+  <si>
+    <t>AN_202105</t>
+  </si>
+  <si>
+    <t>SPI1_202105</t>
+  </si>
+  <si>
+    <t>SPI3_202105</t>
+  </si>
+  <si>
+    <t>SPI6_202105</t>
+  </si>
+  <si>
+    <t>SPI12_202105</t>
   </si>
   <si>
     <t>Pinhal de Sao Bento</t>
@@ -518,8 +518,8 @@
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
@@ -569,31 +569,31 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>-8.8</v>
+        <v>-9.1</v>
       </c>
       <c r="D2">
-        <v>-11.5</v>
+        <v>5.3</v>
       </c>
       <c r="E2">
-        <v>32.3</v>
+        <v>-34</v>
       </c>
       <c r="F2">
-        <v>30.7</v>
+        <v>62.6</v>
       </c>
       <c r="G2">
-        <v>-82.7</v>
+        <v>-64</v>
       </c>
       <c r="H2">
-        <v>3.69</v>
+        <v>-1.27</v>
       </c>
       <c r="I2">
-        <v>1.32</v>
+        <v>-2.84</v>
       </c>
       <c r="J2">
-        <v>0.21</v>
+        <v>-0.69</v>
       </c>
       <c r="K2">
-        <v>-0.32</v>
+        <v>-1.04</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -604,31 +604,31 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>-9.3</v>
+        <v>-11.3</v>
       </c>
       <c r="D3">
-        <v>-20</v>
+        <v>3.6</v>
       </c>
       <c r="E3">
-        <v>30.4</v>
+        <v>-37.4</v>
       </c>
       <c r="F3">
-        <v>43</v>
+        <v>74.6</v>
       </c>
       <c r="G3">
-        <v>-72.9</v>
+        <v>-55.4</v>
       </c>
       <c r="H3">
-        <v>3.66</v>
+        <v>-1.25</v>
       </c>
       <c r="I3">
-        <v>1.29</v>
+        <v>-2.62</v>
       </c>
       <c r="J3">
-        <v>-0.07</v>
+        <v>-0.64</v>
       </c>
       <c r="K3">
-        <v>-0.44</v>
+        <v>-1.03</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -639,31 +639,31 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>5.1</v>
+        <v>-7.1</v>
       </c>
       <c r="D4">
-        <v>7.6</v>
+        <v>12.9</v>
       </c>
       <c r="E4">
-        <v>72.7</v>
+        <v>-62.1</v>
       </c>
       <c r="F4">
-        <v>31.2</v>
+        <v>33.8</v>
       </c>
       <c r="G4">
-        <v>-77.3</v>
+        <v>-74.2</v>
       </c>
       <c r="H4">
-        <v>3.5</v>
+        <v>-1.28</v>
       </c>
       <c r="I4">
-        <v>0.97</v>
+        <v>-3.47</v>
       </c>
       <c r="J4">
-        <v>0.02</v>
+        <v>-0.91</v>
       </c>
       <c r="K4">
-        <v>-0.34</v>
+        <v>-1.1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -674,31 +674,31 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>-5.7</v>
+        <v>-8.8</v>
       </c>
       <c r="D5">
-        <v>-2.5</v>
+        <v>5.4</v>
       </c>
       <c r="E5">
-        <v>40.5</v>
+        <v>-50.5</v>
       </c>
       <c r="F5">
-        <v>18.5</v>
+        <v>48.5</v>
       </c>
       <c r="G5">
-        <v>-88.9</v>
+        <v>-62</v>
       </c>
       <c r="H5">
-        <v>2.66</v>
+        <v>-1.33</v>
       </c>
       <c r="I5">
-        <v>1.24</v>
+        <v>-2.14</v>
       </c>
       <c r="J5">
-        <v>-0.37</v>
+        <v>-0.78</v>
       </c>
       <c r="K5">
-        <v>-0.6</v>
+        <v>-1.27</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -709,31 +709,31 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>-14.1</v>
+        <v>-21.7</v>
       </c>
       <c r="D6">
-        <v>-7.2</v>
+        <v>-0.8</v>
       </c>
       <c r="E6">
-        <v>56.1</v>
+        <v>-64.1</v>
       </c>
       <c r="F6">
-        <v>58.7</v>
+        <v>30.7</v>
       </c>
       <c r="G6">
-        <v>-59</v>
+        <v>-80.7</v>
       </c>
       <c r="H6">
-        <v>4.15</v>
+        <v>-1.37</v>
       </c>
       <c r="I6">
-        <v>-0.22</v>
+        <v>-2.77</v>
       </c>
       <c r="J6">
-        <v>-0.85</v>
+        <v>-2.11</v>
       </c>
       <c r="K6">
-        <v>-1.23</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -744,31 +744,31 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>-27.6</v>
+        <v>-38.9</v>
       </c>
       <c r="D7">
-        <v>-32.1</v>
+        <v>-38.4</v>
       </c>
       <c r="E7">
-        <v>-2.3</v>
+        <v>-79.5</v>
       </c>
       <c r="F7">
-        <v>9.1</v>
+        <v>19.1</v>
       </c>
       <c r="G7">
-        <v>-93.5</v>
+        <v>-88.7</v>
       </c>
       <c r="H7">
-        <v>4.05</v>
+        <v>-1.26</v>
       </c>
       <c r="I7">
-        <v>1.73</v>
+        <v>-2.55</v>
       </c>
       <c r="J7">
-        <v>0.33</v>
+        <v>-0.57</v>
       </c>
       <c r="K7">
-        <v>-0.03</v>
+        <v>-0.98</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -779,31 +779,31 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>-35.5</v>
+        <v>-23.3</v>
       </c>
       <c r="D8">
-        <v>-34.3</v>
+        <v>-20.1</v>
       </c>
       <c r="E8">
-        <v>-21.5</v>
+        <v>-31.5</v>
       </c>
       <c r="F8">
-        <v>67.1</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>-50.9</v>
+        <v>-23.8</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="I8">
-        <v>0.9</v>
+        <v>-0.4</v>
       </c>
       <c r="J8">
-        <v>0.45</v>
+        <v>0.21</v>
       </c>
       <c r="K8">
-        <v>-0.36</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -814,31 +814,31 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>-19</v>
+        <v>-24.6</v>
       </c>
       <c r="D9">
-        <v>-31.1</v>
+        <v>-18.2</v>
       </c>
       <c r="E9">
-        <v>8.7</v>
+        <v>-50.7</v>
       </c>
       <c r="F9">
-        <v>22</v>
+        <v>73.8</v>
       </c>
       <c r="G9">
-        <v>-85.3</v>
+        <v>-57.4</v>
       </c>
       <c r="H9">
-        <v>3.53</v>
+        <v>-1.23</v>
       </c>
       <c r="I9">
-        <v>1.06</v>
+        <v>-2.49</v>
       </c>
       <c r="J9">
-        <v>-0.46</v>
+        <v>-0.61</v>
       </c>
       <c r="K9">
-        <v>-0.72</v>
+        <v>-1.01</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -849,31 +849,31 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>-2.8</v>
+        <v>-4.8</v>
       </c>
       <c r="D10">
-        <v>8.9</v>
+        <v>18.2</v>
       </c>
       <c r="E10">
-        <v>68.5</v>
+        <v>-45.7</v>
       </c>
       <c r="F10">
-        <v>46.1</v>
+        <v>35.8</v>
       </c>
       <c r="G10">
-        <v>-68.1</v>
+        <v>-75.2</v>
       </c>
       <c r="H10">
-        <v>3.12</v>
+        <v>-1.29</v>
       </c>
       <c r="I10">
-        <v>1.2</v>
+        <v>-1.69</v>
       </c>
       <c r="J10">
-        <v>0.17</v>
+        <v>-0.73</v>
       </c>
       <c r="K10">
-        <v>-0.68</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -884,31 +884,31 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>-5</v>
+        <v>-9.9</v>
       </c>
       <c r="D11">
-        <v>-0.2</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>52.8</v>
+        <v>-46.1</v>
       </c>
       <c r="F11">
-        <v>26.3</v>
+        <v>47.2</v>
       </c>
       <c r="G11">
-        <v>-84.8</v>
+        <v>-71.7</v>
       </c>
       <c r="H11">
-        <v>3.73</v>
+        <v>-1.27</v>
       </c>
       <c r="I11">
-        <v>1.42</v>
+        <v>-2.85</v>
       </c>
       <c r="J11">
-        <v>0.47</v>
+        <v>-0.61</v>
       </c>
       <c r="K11">
-        <v>-0.27</v>
+        <v>-1.01</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -919,31 +919,31 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>-4.9</v>
+        <v>-9.2</v>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>55</v>
+        <v>-46.1</v>
       </c>
       <c r="F12">
-        <v>27.3</v>
+        <v>47.3</v>
       </c>
       <c r="G12">
-        <v>-84.4</v>
+        <v>-71.7</v>
       </c>
       <c r="H12">
-        <v>3.71</v>
+        <v>-1.27</v>
       </c>
       <c r="I12">
-        <v>1.39</v>
+        <v>-2.9</v>
       </c>
       <c r="J12">
-        <v>0.43</v>
+        <v>-0.63</v>
       </c>
       <c r="K12">
-        <v>-0.28</v>
+        <v>-1.02</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -954,31 +954,31 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>-7.5</v>
+        <v>-8.6</v>
       </c>
       <c r="D13">
-        <v>-4.9</v>
+        <v>7.3</v>
       </c>
       <c r="E13">
-        <v>41.2</v>
+        <v>-38.8</v>
       </c>
       <c r="F13">
-        <v>26.7</v>
+        <v>59.8</v>
       </c>
       <c r="G13">
-        <v>-85</v>
+        <v>-64.8</v>
       </c>
       <c r="H13">
-        <v>3.74</v>
+        <v>-1.27</v>
       </c>
       <c r="I13">
-        <v>1.39</v>
+        <v>-2.81</v>
       </c>
       <c r="J13">
-        <v>0.31</v>
+        <v>-0.65</v>
       </c>
       <c r="K13">
-        <v>-0.28</v>
+        <v>-1.02</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -989,31 +989,31 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>-22.9</v>
+        <v>-23.6</v>
       </c>
       <c r="D14">
-        <v>-27.3</v>
+        <v>-14.9</v>
       </c>
       <c r="E14">
-        <v>11.6</v>
+        <v>-51.3</v>
       </c>
       <c r="F14">
-        <v>27.4</v>
+        <v>71.6</v>
       </c>
       <c r="G14">
-        <v>-82.6</v>
+        <v>-51.6</v>
       </c>
       <c r="H14">
-        <v>3.01</v>
+        <v>-1.03</v>
       </c>
       <c r="I14">
-        <v>1.01</v>
+        <v>-2.06</v>
       </c>
       <c r="J14">
-        <v>-0.36</v>
+        <v>-0.73</v>
       </c>
       <c r="K14">
-        <v>-0.63</v>
+        <v>-1.06</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1024,31 +1024,31 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>-34.2</v>
+        <v>-29.3</v>
       </c>
       <c r="D15">
-        <v>-41.2</v>
+        <v>-20.1</v>
       </c>
       <c r="E15">
-        <v>-14.9</v>
+        <v>-33.8</v>
       </c>
       <c r="F15">
-        <v>23.9</v>
+        <v>77.6</v>
       </c>
       <c r="G15">
-        <v>-86.2</v>
+        <v>-27.5</v>
       </c>
       <c r="H15">
-        <v>1.38</v>
+        <v>-0.02</v>
       </c>
       <c r="I15">
-        <v>0.48</v>
+        <v>-0.99</v>
       </c>
       <c r="J15">
-        <v>0.17</v>
+        <v>-0.48</v>
       </c>
       <c r="K15">
-        <v>-0.52</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1059,31 +1059,31 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>-6.6</v>
+        <v>-8.3</v>
       </c>
       <c r="D16">
-        <v>-18.2</v>
+        <v>7.4</v>
       </c>
       <c r="E16">
-        <v>33.6</v>
+        <v>-32.4</v>
       </c>
       <c r="F16">
-        <v>51.4</v>
+        <v>77.1</v>
       </c>
       <c r="G16">
-        <v>-66.4</v>
+        <v>-53.4</v>
       </c>
       <c r="H16">
-        <v>3.62</v>
+        <v>-1.25</v>
       </c>
       <c r="I16">
-        <v>1.24</v>
+        <v>-2.59</v>
       </c>
       <c r="J16">
-        <v>-0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="K16">
-        <v>-0.49</v>
+        <v>-1.03</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1094,31 +1094,31 @@
         <v>26</v>
       </c>
       <c r="C17">
-        <v>-20</v>
+        <v>-24.7</v>
       </c>
       <c r="D17">
-        <v>-31.4</v>
+        <v>-16.9</v>
       </c>
       <c r="E17">
-        <v>9.3</v>
+        <v>-51.6</v>
       </c>
       <c r="F17">
-        <v>28.1</v>
+        <v>70.9</v>
       </c>
       <c r="G17">
-        <v>-81.8</v>
+        <v>-60.1</v>
       </c>
       <c r="H17">
-        <v>3.64</v>
+        <v>-1.25</v>
       </c>
       <c r="I17">
-        <v>1.22</v>
+        <v>-2.56</v>
       </c>
       <c r="J17">
-        <v>-0.25</v>
+        <v>-0.61</v>
       </c>
       <c r="K17">
-        <v>-0.54</v>
+        <v>-1.01</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1129,31 +1129,31 @@
         <v>27</v>
       </c>
       <c r="C18">
-        <v>-24.1</v>
+        <v>-31.3</v>
       </c>
       <c r="D18">
-        <v>-22.3</v>
+        <v>-18.3</v>
       </c>
       <c r="E18">
-        <v>22.7</v>
+        <v>-71.9</v>
       </c>
       <c r="F18">
-        <v>19.8</v>
+        <v>24.4</v>
       </c>
       <c r="G18">
-        <v>-88.6</v>
+        <v>-84.9</v>
       </c>
       <c r="H18">
-        <v>3.8</v>
+        <v>-1.26</v>
       </c>
       <c r="I18">
-        <v>1.6</v>
+        <v>-2.7</v>
       </c>
       <c r="J18">
-        <v>0.73</v>
+        <v>-0.47</v>
       </c>
       <c r="K18">
-        <v>-0.25</v>
+        <v>-0.96</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1164,31 +1164,31 @@
         <v>28</v>
       </c>
       <c r="C19">
-        <v>-13.4</v>
+        <v>-18.8</v>
       </c>
       <c r="D19">
-        <v>-12.4</v>
+        <v>-6.1</v>
       </c>
       <c r="E19">
-        <v>27.5</v>
+        <v>-50.7</v>
       </c>
       <c r="F19">
-        <v>19.1</v>
+        <v>51.4</v>
       </c>
       <c r="G19">
-        <v>-89.1</v>
+        <v>-70.2</v>
       </c>
       <c r="H19">
-        <v>3.89</v>
+        <v>-1.26</v>
       </c>
       <c r="I19">
-        <v>1.58</v>
+        <v>-2.61</v>
       </c>
       <c r="J19">
-        <v>0.35</v>
+        <v>-0.57</v>
       </c>
       <c r="K19">
-        <v>-0.17</v>
+        <v>-0.99</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1199,31 +1199,31 @@
         <v>29</v>
       </c>
       <c r="C20">
-        <v>-36.3</v>
+        <v>-22.9</v>
       </c>
       <c r="D20">
-        <v>-27.9</v>
+        <v>-9.9</v>
       </c>
       <c r="E20">
-        <v>-11.5</v>
+        <v>-27</v>
       </c>
       <c r="F20">
-        <v>51.7</v>
+        <v>71.9</v>
       </c>
       <c r="G20">
-        <v>-69.3</v>
+        <v>-36.6</v>
       </c>
       <c r="H20">
-        <v>1.83</v>
+        <v>-0.13</v>
       </c>
       <c r="I20">
-        <v>1.17</v>
+        <v>-1.11</v>
       </c>
       <c r="J20">
-        <v>0.72</v>
+        <v>-0.2</v>
       </c>
       <c r="K20">
-        <v>-0.73</v>
+        <v>-0.41</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1234,31 +1234,31 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>-28.1</v>
+        <v>-22.4</v>
       </c>
       <c r="D21">
-        <v>-38.3</v>
+        <v>-17.4</v>
       </c>
       <c r="E21">
-        <v>-19.8</v>
+        <v>-19.2</v>
       </c>
       <c r="F21">
-        <v>58.5</v>
+        <v>115.1</v>
       </c>
       <c r="G21">
-        <v>-68.5</v>
+        <v>-5.1</v>
       </c>
       <c r="H21">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="I21">
-        <v>0.21</v>
+        <v>-0.37</v>
       </c>
       <c r="J21">
-        <v>-0.06</v>
+        <v>-0.36</v>
       </c>
       <c r="K21">
-        <v>-0.72</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1269,31 +1269,31 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>-42.2</v>
+        <v>-37.6</v>
       </c>
       <c r="D22">
-        <v>-51.6</v>
+        <v>-34.7</v>
       </c>
       <c r="E22">
-        <v>-39.4</v>
+        <v>-32</v>
       </c>
       <c r="F22">
-        <v>43.7</v>
+        <v>117.6</v>
       </c>
       <c r="G22">
-        <v>-81.5</v>
+        <v>-22.5</v>
       </c>
       <c r="H22">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="I22">
-        <v>0.21</v>
+        <v>-0.37</v>
       </c>
       <c r="J22">
-        <v>-0.06</v>
+        <v>-0.36</v>
       </c>
       <c r="K22">
-        <v>-0.72</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1304,31 +1304,31 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>-21.3</v>
+        <v>-30.5</v>
       </c>
       <c r="D23">
-        <v>-20.9</v>
+        <v>-22.2</v>
       </c>
       <c r="E23">
-        <v>20.3</v>
+        <v>-73.4</v>
       </c>
       <c r="F23">
-        <v>13.8</v>
+        <v>24.4</v>
       </c>
       <c r="G23">
-        <v>-90.6</v>
+        <v>-84</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>-1.27</v>
       </c>
       <c r="I23">
-        <v>1.7</v>
+        <v>-2.11</v>
       </c>
       <c r="J23">
-        <v>0.38</v>
+        <v>-0.56</v>
       </c>
       <c r="K23">
-        <v>-0.08</v>
+        <v>-0.98</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1339,31 +1339,31 @@
         <v>32</v>
       </c>
       <c r="C24">
-        <v>-52.6</v>
+        <v>-46.1</v>
       </c>
       <c r="D24">
-        <v>-56.4</v>
+        <v>-44.8</v>
       </c>
       <c r="E24">
-        <v>-46.3</v>
+        <v>-48.9</v>
       </c>
       <c r="F24">
-        <v>38.9</v>
+        <v>74.9</v>
       </c>
       <c r="G24">
-        <v>-79.5</v>
+        <v>-44.9</v>
       </c>
       <c r="H24">
-        <v>-0.44</v>
+        <v>-0.13</v>
       </c>
       <c r="I24">
-        <v>-0.36</v>
+        <v>-0.26</v>
       </c>
       <c r="J24">
-        <v>-0.36</v>
+        <v>-0.61</v>
       </c>
       <c r="K24">
-        <v>-0.82</v>
+        <v>-0.67</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1374,31 +1374,31 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <v>-56</v>
+        <v>-50.7</v>
       </c>
       <c r="D25">
-        <v>-61</v>
+        <v>-51.4</v>
       </c>
       <c r="E25">
-        <v>-53.1</v>
+        <v>-55</v>
       </c>
       <c r="F25">
-        <v>37.5</v>
+        <v>70.7</v>
       </c>
       <c r="G25">
-        <v>-81.1</v>
+        <v>-49.7</v>
       </c>
       <c r="H25">
-        <v>-0.71</v>
+        <v>-0.3</v>
       </c>
       <c r="I25">
-        <v>-0.9</v>
+        <v>-0.28</v>
       </c>
       <c r="J25">
-        <v>-0.59</v>
+        <v>-0.96</v>
       </c>
       <c r="K25">
-        <v>-0.81</v>
+        <v>-0.79</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1409,31 +1409,31 @@
         <v>34</v>
       </c>
       <c r="C26">
-        <v>-51.5</v>
+        <v>-45.8</v>
       </c>
       <c r="D26">
-        <v>-59.1</v>
+        <v>-42.6</v>
       </c>
       <c r="E26">
-        <v>-44.5</v>
+        <v>-47.8</v>
       </c>
       <c r="F26">
-        <v>45</v>
+        <v>65.1</v>
       </c>
       <c r="G26">
-        <v>-77</v>
+        <v>-53.1</v>
       </c>
       <c r="H26">
-        <v>-0.32</v>
+        <v>-0.26</v>
       </c>
       <c r="I26">
-        <v>-1.4</v>
+        <v>-0.61</v>
       </c>
       <c r="J26">
-        <v>-0.83</v>
+        <v>-1.3</v>
       </c>
       <c r="K26">
-        <v>-0.85</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1444,31 +1444,31 @@
         <v>35</v>
       </c>
       <c r="C27">
-        <v>-36</v>
+        <v>-33.3</v>
       </c>
       <c r="D27">
-        <v>-43.8</v>
+        <v>-28.6</v>
       </c>
       <c r="E27">
-        <v>-17.4</v>
+        <v>-47.7</v>
       </c>
       <c r="F27">
-        <v>45.2</v>
+        <v>95.6</v>
       </c>
       <c r="G27">
-        <v>-77</v>
+        <v>-38.4</v>
       </c>
       <c r="H27">
-        <v>3.62</v>
+        <v>-1.16</v>
       </c>
       <c r="I27">
-        <v>1.48</v>
+        <v>-1.07</v>
       </c>
       <c r="J27">
-        <v>0.73</v>
+        <v>0.48</v>
       </c>
       <c r="K27">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1479,31 +1479,31 @@
         <v>36</v>
       </c>
       <c r="C28">
-        <v>-6.7</v>
+        <v>-3.9</v>
       </c>
       <c r="D28">
-        <v>-5</v>
+        <v>12.8</v>
       </c>
       <c r="E28">
-        <v>44.4</v>
+        <v>-35.3</v>
       </c>
       <c r="F28">
-        <v>72.7</v>
+        <v>58.4</v>
       </c>
       <c r="G28">
-        <v>-62.1</v>
+        <v>-64.6</v>
       </c>
       <c r="H28">
-        <v>2.02</v>
+        <v>-1.15</v>
       </c>
       <c r="I28">
-        <v>1.13</v>
+        <v>-1.82</v>
       </c>
       <c r="J28">
-        <v>-0.09</v>
+        <v>-0.7</v>
       </c>
       <c r="K28">
-        <v>-0.66</v>
+        <v>-1.03</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1514,31 +1514,31 @@
         <v>37</v>
       </c>
       <c r="C29">
-        <v>-34.4</v>
+        <v>-30.1</v>
       </c>
       <c r="D29">
-        <v>-40.1</v>
+        <v>-23.7</v>
       </c>
       <c r="E29">
-        <v>-14.8</v>
+        <v>-43.3</v>
       </c>
       <c r="F29">
-        <v>49.3</v>
+        <v>107</v>
       </c>
       <c r="G29">
-        <v>-75</v>
+        <v>-19</v>
       </c>
       <c r="H29">
-        <v>1.33</v>
+        <v>-0.22</v>
       </c>
       <c r="I29">
-        <v>0.55</v>
+        <v>-0.51</v>
       </c>
       <c r="J29">
-        <v>0.11</v>
+        <v>-0.09</v>
       </c>
       <c r="K29">
-        <v>-0.64</v>
+        <v>-0.47</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1549,31 +1549,31 @@
         <v>38</v>
       </c>
       <c r="C30">
-        <v>-19.3</v>
+        <v>-25.6</v>
       </c>
       <c r="D30">
-        <v>-16.2</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>56.9</v>
+        <v>-63.7</v>
       </c>
       <c r="F30">
-        <v>17.1</v>
+        <v>24.3</v>
       </c>
       <c r="G30">
-        <v>-87.5</v>
+        <v>-80.8</v>
       </c>
       <c r="H30">
-        <v>2.08</v>
+        <v>-1.58</v>
       </c>
       <c r="I30">
-        <v>0.75</v>
+        <v>-2.35</v>
       </c>
       <c r="J30">
-        <v>-0.4</v>
+        <v>-0.93</v>
       </c>
       <c r="K30">
-        <v>-1.29</v>
+        <v>-1.86</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1584,31 +1584,31 @@
         <v>39</v>
       </c>
       <c r="C31">
-        <v>-20.3</v>
+        <v>-26.2</v>
       </c>
       <c r="D31">
-        <v>-13.9</v>
+        <v>-1.4</v>
       </c>
       <c r="E31">
-        <v>56.4</v>
+        <v>-64.9</v>
       </c>
       <c r="F31">
-        <v>20.9</v>
+        <v>26.9</v>
       </c>
       <c r="G31">
-        <v>-85</v>
+        <v>-81.2</v>
       </c>
       <c r="H31">
-        <v>2.08</v>
+        <v>-1.58</v>
       </c>
       <c r="I31">
-        <v>0.74</v>
+        <v>-2.36</v>
       </c>
       <c r="J31">
-        <v>-0.41</v>
+        <v>-0.94</v>
       </c>
       <c r="K31">
-        <v>-1.29</v>
+        <v>-1.87</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1619,31 +1619,31 @@
         <v>40</v>
       </c>
       <c r="C32">
-        <v>-38.4</v>
+        <v>-24.1</v>
       </c>
       <c r="D32">
-        <v>-29.8</v>
+        <v>-17.6</v>
       </c>
       <c r="E32">
-        <v>-21.3</v>
+        <v>-28.9</v>
       </c>
       <c r="F32">
-        <v>48.2</v>
+        <v>100.1</v>
       </c>
       <c r="G32">
-        <v>-68.3</v>
+        <v>15.5</v>
       </c>
       <c r="H32">
-        <v>0.25</v>
+        <v>0.58</v>
       </c>
       <c r="I32">
-        <v>0.84</v>
+        <v>-0.52</v>
       </c>
       <c r="J32">
-        <v>0.15</v>
+        <v>-0.46</v>
       </c>
       <c r="K32">
-        <v>-1.45</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1654,31 +1654,31 @@
         <v>41</v>
       </c>
       <c r="C33">
-        <v>-24.2</v>
+        <v>-9.1</v>
       </c>
       <c r="D33">
-        <v>-19.4</v>
+        <v>-0.4</v>
       </c>
       <c r="E33">
-        <v>0.5</v>
+        <v>-17.5</v>
       </c>
       <c r="F33">
-        <v>34.7</v>
+        <v>92.3</v>
       </c>
       <c r="G33">
-        <v>-75.1</v>
+        <v>17.3</v>
       </c>
       <c r="H33">
-        <v>1.15</v>
+        <v>-0.05</v>
       </c>
       <c r="I33">
-        <v>1.04</v>
+        <v>-0.8</v>
       </c>
       <c r="J33">
-        <v>0.43</v>
+        <v>-0.19</v>
       </c>
       <c r="K33">
-        <v>-0.83</v>
+        <v>-0.38</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1689,31 +1689,31 @@
         <v>42</v>
       </c>
       <c r="C34">
-        <v>-38.9</v>
+        <v>-21.7</v>
       </c>
       <c r="D34">
-        <v>-33</v>
+        <v>-7.7</v>
       </c>
       <c r="E34">
-        <v>-10.3</v>
+        <v>-18.9</v>
       </c>
       <c r="F34">
-        <v>56</v>
+        <v>97.6</v>
       </c>
       <c r="G34">
-        <v>-67</v>
+        <v>-11.1</v>
       </c>
       <c r="H34">
-        <v>1.05</v>
+        <v>0.4</v>
       </c>
       <c r="I34">
-        <v>1.28</v>
+        <v>0.01</v>
       </c>
       <c r="J34">
-        <v>0.41</v>
+        <v>0.32</v>
       </c>
       <c r="K34">
-        <v>-0.23</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1724,31 +1724,31 @@
         <v>43</v>
       </c>
       <c r="C35">
-        <v>-43.4</v>
+        <v>-25.4</v>
       </c>
       <c r="D35">
-        <v>-38.5</v>
+        <v>-19.7</v>
       </c>
       <c r="E35">
-        <v>-29.6</v>
+        <v>-26.7</v>
       </c>
       <c r="F35">
-        <v>67.3</v>
+        <v>90.1</v>
       </c>
       <c r="G35">
-        <v>-65</v>
+        <v>-18.2</v>
       </c>
       <c r="H35">
-        <v>0.06</v>
+        <v>0.21</v>
       </c>
       <c r="I35">
-        <v>0.59</v>
+        <v>-0.14</v>
       </c>
       <c r="J35">
-        <v>0.03</v>
+        <v>0.31</v>
       </c>
       <c r="K35">
-        <v>-1.07</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1759,31 +1759,31 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>-38.2</v>
+        <v>-18.8</v>
       </c>
       <c r="D36">
-        <v>-33.7</v>
+        <v>-12</v>
       </c>
       <c r="E36">
-        <v>-31.1</v>
+        <v>-10.5</v>
       </c>
       <c r="F36">
-        <v>59.1</v>
+        <v>108.2</v>
       </c>
       <c r="G36">
-        <v>-69.1</v>
+        <v>-0.8</v>
       </c>
       <c r="H36">
-        <v>-0.31</v>
+        <v>0.39</v>
       </c>
       <c r="I36">
-        <v>0.25</v>
+        <v>-0.08</v>
       </c>
       <c r="J36">
-        <v>-0.18</v>
+        <v>-0.15</v>
       </c>
       <c r="K36">
-        <v>-1.15</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1794,31 +1794,31 @@
         <v>45</v>
       </c>
       <c r="C37">
-        <v>-38</v>
+        <v>-18.5</v>
       </c>
       <c r="D37">
-        <v>-33.9</v>
+        <v>-11.2</v>
       </c>
       <c r="E37">
-        <v>-30.9</v>
+        <v>-8.8</v>
       </c>
       <c r="F37">
-        <v>60.7</v>
+        <v>104.6</v>
       </c>
       <c r="G37">
-        <v>-67.2</v>
+        <v>1.3</v>
       </c>
       <c r="H37">
-        <v>-0.18</v>
+        <v>0.34</v>
       </c>
       <c r="I37">
-        <v>0.3</v>
+        <v>-0.17</v>
       </c>
       <c r="J37">
-        <v>-0.18</v>
+        <v>-0.12</v>
       </c>
       <c r="K37">
-        <v>-1.21</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1829,31 +1829,31 @@
         <v>46</v>
       </c>
       <c r="C38">
-        <v>-45.3</v>
+        <v>-27</v>
       </c>
       <c r="D38">
-        <v>-41</v>
+        <v>-21</v>
       </c>
       <c r="E38">
-        <v>-31.9</v>
+        <v>-23.2</v>
       </c>
       <c r="F38">
-        <v>55.2</v>
+        <v>91.5</v>
       </c>
       <c r="G38">
-        <v>-70</v>
+        <v>-19.1</v>
       </c>
       <c r="H38">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
       <c r="I38">
-        <v>0.62</v>
+        <v>-0.13</v>
       </c>
       <c r="J38">
-        <v>0.06</v>
+        <v>0.29</v>
       </c>
       <c r="K38">
-        <v>-1.04</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1864,31 +1864,31 @@
         <v>47</v>
       </c>
       <c r="C39">
-        <v>-40.6</v>
+        <v>-21.7</v>
       </c>
       <c r="D39">
-        <v>-37.2</v>
+        <v>-14.5</v>
       </c>
       <c r="E39">
-        <v>-31.6</v>
+        <v>-18.7</v>
       </c>
       <c r="F39">
-        <v>82.8</v>
+        <v>92.9</v>
       </c>
       <c r="G39">
-        <v>-61.5</v>
+        <v>-14.7</v>
       </c>
       <c r="H39">
-        <v>0.21</v>
+        <v>0.03</v>
       </c>
       <c r="I39">
-        <v>0.29</v>
+        <v>-0.42</v>
       </c>
       <c r="J39">
-        <v>-0.3</v>
+        <v>0.15</v>
       </c>
       <c r="K39">
-        <v>-1.35</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1899,31 +1899,31 @@
         <v>48</v>
       </c>
       <c r="C40">
-        <v>-49.7</v>
+        <v>-31.8</v>
       </c>
       <c r="D40">
-        <v>-45.5</v>
+        <v>-25.8</v>
       </c>
       <c r="E40">
-        <v>-40</v>
+        <v>-25.9</v>
       </c>
       <c r="F40">
-        <v>60.6</v>
+        <v>95.9</v>
       </c>
       <c r="G40">
-        <v>-75.1</v>
+        <v>-33.9</v>
       </c>
       <c r="H40">
-        <v>0.02</v>
+        <v>0.26</v>
       </c>
       <c r="I40">
-        <v>0.68</v>
+        <v>-0.02</v>
       </c>
       <c r="J40">
-        <v>0.13</v>
+        <v>0.69</v>
       </c>
       <c r="K40">
-        <v>-0.95</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1934,31 +1934,31 @@
         <v>49</v>
       </c>
       <c r="C41">
-        <v>-34.5</v>
+        <v>-20.6</v>
       </c>
       <c r="D41">
-        <v>-27.7</v>
+        <v>-16</v>
       </c>
       <c r="E41">
-        <v>-17.6</v>
+        <v>-33.5</v>
       </c>
       <c r="F41">
-        <v>60.4</v>
+        <v>91.2</v>
       </c>
       <c r="G41">
-        <v>-55.2</v>
+        <v>-1.8</v>
       </c>
       <c r="H41">
-        <v>0.19</v>
+        <v>0.57</v>
       </c>
       <c r="I41">
-        <v>0.78</v>
+        <v>-0.49</v>
       </c>
       <c r="J41">
-        <v>0.12</v>
+        <v>-0.44</v>
       </c>
       <c r="K41">
-        <v>-1.44</v>
+        <v>-0.47</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1969,31 +1969,31 @@
         <v>50</v>
       </c>
       <c r="C42">
-        <v>-20.5</v>
+        <v>-26.5</v>
       </c>
       <c r="D42">
-        <v>-15.2</v>
+        <v>-7.3</v>
       </c>
       <c r="E42">
-        <v>43.8</v>
+        <v>-65.3</v>
       </c>
       <c r="F42">
-        <v>33.2</v>
+        <v>26.7</v>
       </c>
       <c r="G42">
-        <v>-77.8</v>
+        <v>-82.5</v>
       </c>
       <c r="H42">
-        <v>4.34</v>
+        <v>-1.36</v>
       </c>
       <c r="I42">
-        <v>-0.49</v>
+        <v>-2.7</v>
       </c>
       <c r="J42">
-        <v>-1.04</v>
+        <v>-2.41</v>
       </c>
       <c r="K42">
-        <v>-1.38</v>
+        <v>-2.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>